<commit_message>
Updated simulation to run algorithms
Each algorithm file should be placed in the scq_betting folder. To be executed in the simulation it should be added to the list in main
</commit_message>
<xml_diff>
--- a/__data__/MasterStats.xlsx
+++ b/__data__/MasterStats.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,34 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -453,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG33"/>
+  <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,3430 +434,3451 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0_level_0</t>
+          <t>Unnamed: 0</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 1_level_0</t>
+          <t>Rk</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 2_level_0</t>
+          <t>Season</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 3_level_0</t>
+          <t>Team</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pace</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ORtg</t>
+        </is>
+      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 7_level_0</t>
+          <t>DRtg</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 8_level_0</t>
+          <t>TS%</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 9_level_0</t>
+          <t>TOV%</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 10_level_0</t>
+          <t>FT%</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 11_level_0</t>
+          <t>G</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 12_level_0</t>
+          <t>W.1</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 13_level_0</t>
+          <t>L</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="1" t="n"/>
-      <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="n"/>
-      <c r="U1" s="1" t="n"/>
+          <t>W/L%</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>MOV</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>SOS</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>SRS</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Pace.1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ORtg.1</t>
+        </is>
+      </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Team Shooting</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="n"/>
+          <t>DRtg.1</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>eFG%</t>
+        </is>
+      </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Team</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="n"/>
-      <c r="Z1" s="1" t="n"/>
-      <c r="AA1" s="1" t="n"/>
+          <t>TS%.1</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>TOV%.1</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ORB%</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>DRB%</t>
+        </is>
+      </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Opponent Shooting</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="n"/>
+          <t>FTr</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>eFG%.1</t>
+        </is>
+      </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Opponent</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="n"/>
-      <c r="AF1" s="1" t="n"/>
-      <c r="AG1" s="1" t="n"/>
+          <t>TS%.2</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>TOV%.2</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>ORB%.1</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>DRB%.1</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>FTr.1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Rk</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>Season</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Team</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>Pace</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>ORtg</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>DRtg</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>TS%</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>TOV%</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>FT%</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>W/L%</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>MOV</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>SOS</t>
-        </is>
-      </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>SRS</t>
-        </is>
-      </c>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t>Pace.1</t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr">
-        <is>
-          <t>ORtg.1</t>
-        </is>
-      </c>
-      <c r="U2" s="1" t="inlineStr">
-        <is>
-          <t>DRtg.1</t>
-        </is>
-      </c>
-      <c r="V2" s="1" t="inlineStr">
-        <is>
-          <t>eFG%</t>
-        </is>
-      </c>
-      <c r="W2" s="1" t="inlineStr">
-        <is>
-          <t>TS%</t>
-        </is>
-      </c>
-      <c r="X2" s="1" t="inlineStr">
-        <is>
-          <t>TOV%</t>
-        </is>
-      </c>
-      <c r="Y2" s="1" t="inlineStr">
-        <is>
-          <t>ORB%</t>
-        </is>
-      </c>
-      <c r="Z2" s="1" t="inlineStr">
-        <is>
-          <t>DRB%</t>
-        </is>
-      </c>
-      <c r="AA2" s="1" t="inlineStr">
-        <is>
-          <t>FTr</t>
-        </is>
-      </c>
-      <c r="AB2" s="1" t="inlineStr">
-        <is>
-          <t>eFG%</t>
-        </is>
-      </c>
-      <c r="AC2" s="1" t="inlineStr">
-        <is>
-          <t>TS%</t>
-        </is>
-      </c>
-      <c r="AD2" s="1" t="inlineStr">
-        <is>
-          <t>TOV%</t>
-        </is>
-      </c>
-      <c r="AE2" s="1" t="inlineStr">
-        <is>
-          <t>ORB%</t>
-        </is>
-      </c>
-      <c r="AF2" s="1" t="inlineStr">
-        <is>
-          <t>DRB%</t>
-        </is>
-      </c>
-      <c r="AG2" s="1" t="inlineStr">
-        <is>
-          <t>FTr</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>BOS</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>64</v>
+      </c>
+      <c r="G3" t="n">
+        <v>97.2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>123.2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>111.6</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="K3" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="M3" t="n">
+        <v>82</v>
+      </c>
+      <c r="N3" t="n">
+        <v>64</v>
+      </c>
+      <c r="O3" t="n">
+        <v>18</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>11.34</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="S3" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="T3" t="n">
+        <v>97.2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>123.2</v>
+      </c>
+      <c r="V3" t="n">
+        <v>111.6</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.578</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>24.9</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>76.3</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.189</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>BOS</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>64</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>OKC</t>
+        </is>
       </c>
       <c r="F4" t="n">
-        <v>97.2</v>
+        <v>57</v>
       </c>
       <c r="G4" t="n">
-        <v>123.2</v>
+        <v>99.8</v>
       </c>
       <c r="H4" t="n">
-        <v>111.6</v>
+        <v>119.5</v>
       </c>
       <c r="I4" t="n">
-        <v>0.609</v>
+        <v>112.1</v>
       </c>
       <c r="J4" t="n">
-        <v>10.8</v>
+        <v>0.608</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8070000000000001</v>
+        <v>11.4</v>
       </c>
       <c r="L4" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="M4" t="n">
         <v>82</v>
       </c>
-      <c r="M4" t="n">
-        <v>64</v>
-      </c>
       <c r="N4" t="n">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="O4" t="n">
-        <v>0.78</v>
+        <v>25</v>
       </c>
       <c r="P4" t="n">
-        <v>11.34</v>
+        <v>0.695</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.6</v>
+        <v>7.41</v>
       </c>
       <c r="R4" t="n">
-        <v>10.75</v>
+        <v>-0.05</v>
       </c>
       <c r="S4" t="n">
-        <v>97.2</v>
+        <v>7.36</v>
       </c>
       <c r="T4" t="n">
-        <v>123.2</v>
+        <v>99.8</v>
       </c>
       <c r="U4" t="n">
-        <v>111.6</v>
+        <v>119.5</v>
       </c>
       <c r="V4" t="n">
-        <v>0.578</v>
+        <v>112.1</v>
       </c>
       <c r="W4" t="n">
-        <v>0.609</v>
+        <v>0.573</v>
       </c>
       <c r="X4" t="n">
-        <v>10.8</v>
+        <v>0.608</v>
       </c>
       <c r="Y4" t="n">
-        <v>24.9</v>
+        <v>11.4</v>
       </c>
       <c r="Z4" t="n">
-        <v>76.3</v>
+        <v>21.1</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.224</v>
+        <v>73.8</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.523</v>
+        <v>0.24</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
       <c r="AD4" t="n">
-        <v>10.8</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="AE4" t="n">
-        <v>23.7</v>
+        <v>13.6</v>
       </c>
       <c r="AF4" t="n">
-        <v>75.09999999999999</v>
+        <v>26.2</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.189</v>
+        <v>78.90000000000001</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0.256</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>2</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>OKC</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
         <v>57</v>
       </c>
-      <c r="F5" t="n">
-        <v>99.8</v>
-      </c>
       <c r="G5" t="n">
-        <v>119.5</v>
+        <v>96.8</v>
       </c>
       <c r="H5" t="n">
-        <v>112.1</v>
+        <v>118.5</v>
       </c>
       <c r="I5" t="n">
-        <v>0.608</v>
+        <v>113</v>
       </c>
       <c r="J5" t="n">
-        <v>11.4</v>
+        <v>0.589</v>
       </c>
       <c r="K5" t="n">
-        <v>0.825</v>
+        <v>11.5</v>
       </c>
       <c r="L5" t="n">
+        <v>0.762</v>
+      </c>
+      <c r="M5" t="n">
         <v>82</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>57</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>25</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>0.695</v>
       </c>
-      <c r="P5" t="n">
-        <v>7.41</v>
-      </c>
       <c r="Q5" t="n">
-        <v>-0.05</v>
+        <v>5.26</v>
       </c>
       <c r="R5" t="n">
-        <v>7.36</v>
+        <v>-0.03</v>
       </c>
       <c r="S5" t="n">
-        <v>99.8</v>
+        <v>5.23</v>
       </c>
       <c r="T5" t="n">
-        <v>119.5</v>
+        <v>96.8</v>
       </c>
       <c r="U5" t="n">
-        <v>112.1</v>
+        <v>118.5</v>
       </c>
       <c r="V5" t="n">
-        <v>0.573</v>
+        <v>113</v>
       </c>
       <c r="W5" t="n">
-        <v>0.608</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="X5" t="n">
-        <v>11.4</v>
+        <v>0.589</v>
       </c>
       <c r="Y5" t="n">
-        <v>21.1</v>
+        <v>11.5</v>
       </c>
       <c r="Z5" t="n">
-        <v>73.8</v>
+        <v>25.5</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.24</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.53</v>
+        <v>0.224</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.526</v>
       </c>
       <c r="AD5" t="n">
-        <v>13.6</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="AE5" t="n">
-        <v>26.2</v>
+        <v>11.2</v>
       </c>
       <c r="AF5" t="n">
-        <v>78.90000000000001</v>
+        <v>24.4</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.256</v>
+        <v>74.5</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.252</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>3</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>DEN</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>57</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
       </c>
       <c r="F6" t="n">
-        <v>96.8</v>
+        <v>56</v>
       </c>
       <c r="G6" t="n">
-        <v>118.5</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>113</v>
+        <v>115.6</v>
       </c>
       <c r="I6" t="n">
-        <v>0.589</v>
+        <v>109</v>
       </c>
       <c r="J6" t="n">
-        <v>11.5</v>
+        <v>0.594</v>
       </c>
       <c r="K6" t="n">
-        <v>0.762</v>
+        <v>13</v>
       </c>
       <c r="L6" t="n">
+        <v>0.777</v>
+      </c>
+      <c r="M6" t="n">
         <v>82</v>
       </c>
-      <c r="M6" t="n">
-        <v>57</v>
-      </c>
       <c r="N6" t="n">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="O6" t="n">
-        <v>0.695</v>
+        <v>26</v>
       </c>
       <c r="P6" t="n">
-        <v>5.26</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.03</v>
+        <v>6.45</v>
       </c>
       <c r="R6" t="n">
-        <v>5.23</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="S6" t="n">
-        <v>96.8</v>
+        <v>6.39</v>
       </c>
       <c r="T6" t="n">
-        <v>118.5</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="U6" t="n">
-        <v>113</v>
+        <v>115.6</v>
       </c>
       <c r="V6" t="n">
-        <v>0.5620000000000001</v>
+        <v>109</v>
       </c>
       <c r="W6" t="n">
-        <v>0.589</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="X6" t="n">
-        <v>11.5</v>
+        <v>0.594</v>
       </c>
       <c r="Y6" t="n">
-        <v>25.5</v>
+        <v>13</v>
       </c>
       <c r="Z6" t="n">
-        <v>75.59999999999999</v>
+        <v>23.2</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.224</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.526</v>
+        <v>0.27</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.515</v>
       </c>
       <c r="AD6" t="n">
-        <v>11.2</v>
+        <v>0.553</v>
       </c>
       <c r="AE6" t="n">
-        <v>24.4</v>
+        <v>12.9</v>
       </c>
       <c r="AF6" t="n">
-        <v>74.5</v>
+        <v>23.1</v>
       </c>
       <c r="AG6" t="n">
+        <v>76.8</v>
+      </c>
+      <c r="AH6" t="n">
         <v>0.252</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>4</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>56</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
       </c>
       <c r="F7" t="n">
-        <v>97.09999999999999</v>
+        <v>51</v>
       </c>
       <c r="G7" t="n">
-        <v>115.6</v>
+        <v>97.2</v>
       </c>
       <c r="H7" t="n">
-        <v>109</v>
+        <v>118.8</v>
       </c>
       <c r="I7" t="n">
-        <v>0.594</v>
+        <v>115.4</v>
       </c>
       <c r="J7" t="n">
-        <v>13</v>
+        <v>0.599</v>
       </c>
       <c r="K7" t="n">
-        <v>0.777</v>
+        <v>12</v>
       </c>
       <c r="L7" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="M7" t="n">
         <v>82</v>
       </c>
-      <c r="M7" t="n">
-        <v>56</v>
-      </c>
       <c r="N7" t="n">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="O7" t="n">
-        <v>0.6830000000000001</v>
+        <v>31</v>
       </c>
       <c r="P7" t="n">
-        <v>6.45</v>
+        <v>0.622</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.07000000000000001</v>
+        <v>3.28</v>
       </c>
       <c r="R7" t="n">
-        <v>6.39</v>
+        <v>0.13</v>
       </c>
       <c r="S7" t="n">
-        <v>97.09999999999999</v>
+        <v>3.41</v>
       </c>
       <c r="T7" t="n">
-        <v>115.6</v>
+        <v>97.2</v>
       </c>
       <c r="U7" t="n">
-        <v>109</v>
+        <v>118.8</v>
       </c>
       <c r="V7" t="n">
-        <v>0.5590000000000001</v>
+        <v>115.4</v>
       </c>
       <c r="W7" t="n">
-        <v>0.594</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="X7" t="n">
-        <v>13</v>
+        <v>0.599</v>
       </c>
       <c r="Y7" t="n">
-        <v>23.2</v>
+        <v>12</v>
       </c>
       <c r="Z7" t="n">
-        <v>76.90000000000001</v>
+        <v>24.4</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.27</v>
+        <v>74.8</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.515</v>
+        <v>0.256</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.553</v>
+        <v>0.541</v>
       </c>
       <c r="AD7" t="n">
-        <v>12.9</v>
+        <v>0.573</v>
       </c>
       <c r="AE7" t="n">
-        <v>23.1</v>
+        <v>11.7</v>
       </c>
       <c r="AF7" t="n">
-        <v>76.8</v>
+        <v>25.2</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.252</v>
+        <v>75.59999999999999</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>0.236</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>LAC</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>51</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NYK</t>
+        </is>
       </c>
       <c r="F8" t="n">
-        <v>97.2</v>
+        <v>50</v>
       </c>
       <c r="G8" t="n">
-        <v>118.8</v>
+        <v>95.2</v>
       </c>
       <c r="H8" t="n">
-        <v>115.4</v>
+        <v>118.2</v>
       </c>
       <c r="I8" t="n">
-        <v>0.599</v>
+        <v>113.4</v>
       </c>
       <c r="J8" t="n">
-        <v>12</v>
+        <v>0.574</v>
       </c>
       <c r="K8" t="n">
-        <v>0.825</v>
+        <v>11.9</v>
       </c>
       <c r="L8" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M8" t="n">
         <v>82</v>
       </c>
-      <c r="M8" t="n">
-        <v>51</v>
-      </c>
       <c r="N8" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="O8" t="n">
-        <v>0.622</v>
+        <v>32</v>
       </c>
       <c r="P8" t="n">
-        <v>3.28</v>
+        <v>0.61</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.13</v>
+        <v>4.59</v>
       </c>
       <c r="R8" t="n">
-        <v>3.41</v>
+        <v>-0.23</v>
       </c>
       <c r="S8" t="n">
-        <v>97.2</v>
+        <v>4.36</v>
       </c>
       <c r="T8" t="n">
-        <v>118.8</v>
+        <v>95.2</v>
       </c>
       <c r="U8" t="n">
-        <v>115.4</v>
+        <v>118.2</v>
       </c>
       <c r="V8" t="n">
-        <v>0.5610000000000001</v>
+        <v>113.4</v>
       </c>
       <c r="W8" t="n">
-        <v>0.599</v>
+        <v>0.54</v>
       </c>
       <c r="X8" t="n">
-        <v>12</v>
+        <v>0.574</v>
       </c>
       <c r="Y8" t="n">
-        <v>24.4</v>
+        <v>11.9</v>
       </c>
       <c r="Z8" t="n">
-        <v>74.8</v>
+        <v>29.4</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.256</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.541</v>
+        <v>0.246</v>
       </c>
       <c r="AC8" t="n">
+        <v>0.543</v>
+      </c>
+      <c r="AD8" t="n">
         <v>0.573</v>
       </c>
-      <c r="AD8" t="n">
-        <v>11.7</v>
-      </c>
       <c r="AE8" t="n">
-        <v>25.2</v>
+        <v>12.3</v>
       </c>
       <c r="AF8" t="n">
-        <v>75.59999999999999</v>
+        <v>23.9</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.236</v>
+        <v>70.59999999999999</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>0.231</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>6</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NYK</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>50</v>
       </c>
-      <c r="F9" t="n">
-        <v>95.2</v>
-      </c>
       <c r="G9" t="n">
-        <v>118.2</v>
+        <v>100.1</v>
       </c>
       <c r="H9" t="n">
-        <v>113.4</v>
+        <v>117.6</v>
       </c>
       <c r="I9" t="n">
-        <v>0.574</v>
+        <v>115.4</v>
       </c>
       <c r="J9" t="n">
-        <v>11.9</v>
+        <v>0.592</v>
       </c>
       <c r="K9" t="n">
-        <v>0.78</v>
+        <v>11.2</v>
       </c>
       <c r="L9" t="n">
+        <v>0.758</v>
+      </c>
+      <c r="M9" t="n">
         <v>82</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>50</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>32</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>0.61</v>
       </c>
-      <c r="P9" t="n">
-        <v>4.59</v>
-      </c>
       <c r="Q9" t="n">
-        <v>-0.23</v>
+        <v>2.21</v>
       </c>
       <c r="R9" t="n">
-        <v>4.36</v>
+        <v>0.09</v>
       </c>
       <c r="S9" t="n">
-        <v>95.2</v>
+        <v>2.3</v>
       </c>
       <c r="T9" t="n">
-        <v>118.2</v>
+        <v>100.1</v>
       </c>
       <c r="U9" t="n">
-        <v>113.4</v>
+        <v>117.6</v>
       </c>
       <c r="V9" t="n">
-        <v>0.54</v>
+        <v>115.4</v>
       </c>
       <c r="W9" t="n">
-        <v>0.574</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="X9" t="n">
-        <v>11.9</v>
+        <v>0.592</v>
       </c>
       <c r="Y9" t="n">
-        <v>29.4</v>
+        <v>11.2</v>
       </c>
       <c r="Z9" t="n">
-        <v>76.09999999999999</v>
+        <v>22.2</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.246</v>
+        <v>75.2</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.543</v>
+        <v>0.251</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.573</v>
+        <v>0.548</v>
       </c>
       <c r="AD9" t="n">
-        <v>12.3</v>
+        <v>0.579</v>
       </c>
       <c r="AE9" t="n">
-        <v>23.9</v>
+        <v>12.1</v>
       </c>
       <c r="AF9" t="n">
-        <v>70.59999999999999</v>
+        <v>24.8</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.231</v>
+        <v>77.8</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>0.239</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>7</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>50</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
       </c>
       <c r="F10" t="n">
-        <v>100.1</v>
+        <v>49</v>
       </c>
       <c r="G10" t="n">
-        <v>117.6</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>115.4</v>
+        <v>118.4</v>
       </c>
       <c r="I10" t="n">
-        <v>0.592</v>
+        <v>115.8</v>
       </c>
       <c r="J10" t="n">
-        <v>11.2</v>
+        <v>0.601</v>
       </c>
       <c r="K10" t="n">
-        <v>0.758</v>
+        <v>11.5</v>
       </c>
       <c r="L10" t="n">
+        <v>0.774</v>
+      </c>
+      <c r="M10" t="n">
         <v>82</v>
       </c>
-      <c r="M10" t="n">
-        <v>50</v>
-      </c>
       <c r="N10" t="n">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="O10" t="n">
-        <v>0.61</v>
+        <v>33</v>
       </c>
       <c r="P10" t="n">
-        <v>2.21</v>
+        <v>0.598</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.09</v>
+        <v>2.62</v>
       </c>
       <c r="R10" t="n">
-        <v>2.3</v>
+        <v>-0.18</v>
       </c>
       <c r="S10" t="n">
-        <v>100.1</v>
+        <v>2.44</v>
       </c>
       <c r="T10" t="n">
-        <v>117.6</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="U10" t="n">
-        <v>115.4</v>
+        <v>118.4</v>
       </c>
       <c r="V10" t="n">
-        <v>0.5620000000000001</v>
+        <v>115.8</v>
       </c>
       <c r="W10" t="n">
-        <v>0.592</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="X10" t="n">
-        <v>11.2</v>
+        <v>0.601</v>
       </c>
       <c r="Y10" t="n">
-        <v>22.2</v>
+        <v>11.5</v>
       </c>
       <c r="Z10" t="n">
-        <v>75.2</v>
+        <v>21.8</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.251</v>
+        <v>77.2</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.548</v>
+        <v>0.27</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.579</v>
+        <v>0.539</v>
       </c>
       <c r="AD10" t="n">
-        <v>12.1</v>
+        <v>0.574</v>
       </c>
       <c r="AE10" t="n">
-        <v>24.8</v>
+        <v>10.6</v>
       </c>
       <c r="AF10" t="n">
-        <v>77.8</v>
+        <v>22.8</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.239</v>
+        <v>78.2</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>0.234</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>8</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>MIL</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>PHO</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
         <v>49</v>
       </c>
-      <c r="F11" t="n">
-        <v>99.90000000000001</v>
-      </c>
       <c r="G11" t="n">
-        <v>118.4</v>
+        <v>98.3</v>
       </c>
       <c r="H11" t="n">
-        <v>115.8</v>
+        <v>117.6</v>
       </c>
       <c r="I11" t="n">
-        <v>0.601</v>
+        <v>114.6</v>
       </c>
       <c r="J11" t="n">
-        <v>11.5</v>
+        <v>0.603</v>
       </c>
       <c r="K11" t="n">
-        <v>0.774</v>
+        <v>13.4</v>
       </c>
       <c r="L11" t="n">
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="M11" t="n">
         <v>82</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>49</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>33</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>0.598</v>
       </c>
-      <c r="P11" t="n">
-        <v>2.62</v>
-      </c>
       <c r="Q11" t="n">
-        <v>-0.18</v>
+        <v>3.06</v>
       </c>
       <c r="R11" t="n">
-        <v>2.44</v>
+        <v>0.02</v>
       </c>
       <c r="S11" t="n">
-        <v>99.90000000000001</v>
+        <v>3.08</v>
       </c>
       <c r="T11" t="n">
-        <v>118.4</v>
+        <v>98.3</v>
       </c>
       <c r="U11" t="n">
-        <v>115.8</v>
+        <v>117.6</v>
       </c>
       <c r="V11" t="n">
-        <v>0.5679999999999999</v>
+        <v>114.6</v>
       </c>
       <c r="W11" t="n">
-        <v>0.601</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="X11" t="n">
-        <v>11.5</v>
+        <v>0.603</v>
       </c>
       <c r="Y11" t="n">
-        <v>21.8</v>
+        <v>13.4</v>
       </c>
       <c r="Z11" t="n">
-        <v>77.2</v>
+        <v>25</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.27</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.539</v>
+        <v>0.271</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.574</v>
+        <v>0.536</v>
       </c>
       <c r="AD11" t="n">
-        <v>10.6</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="AE11" t="n">
-        <v>22.8</v>
+        <v>11.3</v>
       </c>
       <c r="AF11" t="n">
-        <v>78.2</v>
+        <v>24.4</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.234</v>
+        <v>75</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>0.23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>9</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>PHO</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>NOP</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>49</v>
       </c>
-      <c r="F12" t="n">
-        <v>98.3</v>
-      </c>
       <c r="G12" t="n">
-        <v>117.6</v>
+        <v>97.90000000000001</v>
       </c>
       <c r="H12" t="n">
-        <v>114.6</v>
+        <v>117.4</v>
       </c>
       <c r="I12" t="n">
-        <v>0.603</v>
+        <v>112.9</v>
       </c>
       <c r="J12" t="n">
-        <v>13.4</v>
+        <v>0.591</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8080000000000001</v>
+        <v>11.8</v>
       </c>
       <c r="L12" t="n">
+        <v>0.771</v>
+      </c>
+      <c r="M12" t="n">
         <v>82</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>49</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>33</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>0.598</v>
       </c>
-      <c r="P12" t="n">
-        <v>3.06</v>
-      </c>
       <c r="Q12" t="n">
-        <v>0.02</v>
+        <v>4.41</v>
       </c>
       <c r="R12" t="n">
-        <v>3.08</v>
+        <v>0.05</v>
       </c>
       <c r="S12" t="n">
-        <v>98.3</v>
+        <v>4.46</v>
       </c>
       <c r="T12" t="n">
-        <v>117.6</v>
+        <v>97.90000000000001</v>
       </c>
       <c r="U12" t="n">
-        <v>114.6</v>
+        <v>117.4</v>
       </c>
       <c r="V12" t="n">
-        <v>0.5649999999999999</v>
+        <v>112.9</v>
       </c>
       <c r="W12" t="n">
-        <v>0.603</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="X12" t="n">
-        <v>13.4</v>
+        <v>0.591</v>
       </c>
       <c r="Y12" t="n">
-        <v>25</v>
+        <v>11.8</v>
       </c>
       <c r="Z12" t="n">
+        <v>24.4</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>76.90000000000001</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.541</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="AG12" t="n">
         <v>75.59999999999999</v>
       </c>
-      <c r="AA12" t="n">
-        <v>0.271</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>0.536</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>0.5669999999999999</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>24.4</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>75</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>0.23</v>
+      <c r="AH12" t="n">
+        <v>0.237</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>10</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>NOP</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>49</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
       </c>
       <c r="F13" t="n">
-        <v>97.90000000000001</v>
+        <v>48</v>
       </c>
       <c r="G13" t="n">
-        <v>117.4</v>
+        <v>97.2</v>
       </c>
       <c r="H13" t="n">
-        <v>112.9</v>
+        <v>115.2</v>
       </c>
       <c r="I13" t="n">
-        <v>0.591</v>
+        <v>112.7</v>
       </c>
       <c r="J13" t="n">
-        <v>11.8</v>
+        <v>0.586</v>
       </c>
       <c r="K13" t="n">
-        <v>0.771</v>
+        <v>12.4</v>
       </c>
       <c r="L13" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="M13" t="n">
         <v>82</v>
       </c>
-      <c r="M13" t="n">
-        <v>49</v>
-      </c>
       <c r="N13" t="n">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="O13" t="n">
-        <v>0.598</v>
+        <v>34</v>
       </c>
       <c r="P13" t="n">
-        <v>4.41</v>
+        <v>0.585</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.05</v>
+        <v>2.41</v>
       </c>
       <c r="R13" t="n">
-        <v>4.46</v>
+        <v>-0.44</v>
       </c>
       <c r="S13" t="n">
-        <v>97.90000000000001</v>
+        <v>1.98</v>
       </c>
       <c r="T13" t="n">
-        <v>117.4</v>
+        <v>97.2</v>
       </c>
       <c r="U13" t="n">
-        <v>112.9</v>
+        <v>115.2</v>
       </c>
       <c r="V13" t="n">
-        <v>0.5580000000000001</v>
+        <v>112.7</v>
       </c>
       <c r="W13" t="n">
-        <v>0.591</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="X13" t="n">
-        <v>11.8</v>
+        <v>0.586</v>
       </c>
       <c r="Y13" t="n">
-        <v>24.4</v>
+        <v>12.4</v>
       </c>
       <c r="Z13" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="AA13" t="n">
         <v>76.90000000000001</v>
       </c>
-      <c r="AA13" t="n">
-        <v>0.261</v>
-      </c>
       <c r="AB13" t="n">
-        <v>0.541</v>
+        <v>0.234</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.574</v>
+        <v>0.535</v>
       </c>
       <c r="AD13" t="n">
-        <v>12.9</v>
+        <v>0.57</v>
       </c>
       <c r="AE13" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="AF13" t="n">
         <v>23.1</v>
       </c>
-      <c r="AF13" t="n">
-        <v>75.59999999999999</v>
-      </c>
       <c r="AG13" t="n">
-        <v>0.237</v>
+        <v>76.8</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>0.24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>11</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>CLE</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>48</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
       </c>
       <c r="F14" t="n">
-        <v>97.2</v>
+        <v>47</v>
       </c>
       <c r="G14" t="n">
-        <v>115.2</v>
+        <v>100.9</v>
       </c>
       <c r="H14" t="n">
-        <v>112.7</v>
+        <v>115.9</v>
       </c>
       <c r="I14" t="n">
-        <v>0.586</v>
+        <v>115.3</v>
       </c>
       <c r="J14" t="n">
-        <v>12.4</v>
+        <v>0.601</v>
       </c>
       <c r="K14" t="n">
-        <v>0.765</v>
+        <v>12.5</v>
       </c>
       <c r="L14" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="M14" t="n">
         <v>82</v>
       </c>
-      <c r="M14" t="n">
-        <v>48</v>
-      </c>
       <c r="N14" t="n">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="O14" t="n">
-        <v>0.585</v>
+        <v>35</v>
       </c>
       <c r="P14" t="n">
-        <v>2.41</v>
+        <v>0.573</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.44</v>
+        <v>0.6</v>
       </c>
       <c r="R14" t="n">
-        <v>1.98</v>
+        <v>0.48</v>
       </c>
       <c r="S14" t="n">
-        <v>97.2</v>
+        <v>1.07</v>
       </c>
       <c r="T14" t="n">
-        <v>115.2</v>
+        <v>100.9</v>
       </c>
       <c r="U14" t="n">
-        <v>112.7</v>
+        <v>115.9</v>
       </c>
       <c r="V14" t="n">
-        <v>0.5570000000000001</v>
+        <v>115.3</v>
       </c>
       <c r="W14" t="n">
-        <v>0.586</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="X14" t="n">
-        <v>12.4</v>
+        <v>0.601</v>
       </c>
       <c r="Y14" t="n">
-        <v>23.2</v>
+        <v>12.5</v>
       </c>
       <c r="Z14" t="n">
-        <v>76.90000000000001</v>
+        <v>19.9</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.234</v>
+        <v>76.2</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.535</v>
+        <v>0.276</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.57</v>
+        <v>0.55</v>
       </c>
       <c r="AD14" t="n">
-        <v>12.3</v>
+        <v>0.578</v>
       </c>
       <c r="AE14" t="n">
-        <v>23.1</v>
+        <v>11.7</v>
       </c>
       <c r="AF14" t="n">
-        <v>76.8</v>
+        <v>23.8</v>
       </c>
       <c r="AG14" t="n">
-        <v>0.24</v>
+        <v>80.09999999999999</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>0.192</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>12</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>LAL</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>47</v>
       </c>
-      <c r="F15" t="n">
-        <v>100.9</v>
-      </c>
       <c r="G15" t="n">
-        <v>115.9</v>
+        <v>97.5</v>
       </c>
       <c r="H15" t="n">
-        <v>115.3</v>
+        <v>116.9</v>
       </c>
       <c r="I15" t="n">
-        <v>0.601</v>
+        <v>113.8</v>
       </c>
       <c r="J15" t="n">
-        <v>12.5</v>
+        <v>0.574</v>
       </c>
       <c r="K15" t="n">
-        <v>0.782</v>
+        <v>10.7</v>
       </c>
       <c r="L15" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="M15" t="n">
         <v>82</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>47</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>35</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>0.573</v>
       </c>
-      <c r="P15" t="n">
-        <v>0.6</v>
-      </c>
       <c r="Q15" t="n">
-        <v>0.48</v>
+        <v>3.05</v>
       </c>
       <c r="R15" t="n">
-        <v>1.07</v>
+        <v>-0.54</v>
       </c>
       <c r="S15" t="n">
-        <v>100.9</v>
+        <v>2.51</v>
       </c>
       <c r="T15" t="n">
-        <v>115.9</v>
+        <v>97.5</v>
       </c>
       <c r="U15" t="n">
-        <v>115.3</v>
+        <v>116.9</v>
       </c>
       <c r="V15" t="n">
-        <v>0.5659999999999999</v>
+        <v>113.8</v>
       </c>
       <c r="W15" t="n">
-        <v>0.601</v>
+        <v>0.532</v>
       </c>
       <c r="X15" t="n">
-        <v>12.5</v>
+        <v>0.574</v>
       </c>
       <c r="Y15" t="n">
-        <v>19.9</v>
+        <v>10.7</v>
       </c>
       <c r="Z15" t="n">
-        <v>76.2</v>
+        <v>24.8</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.276</v>
+        <v>74.3</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.55</v>
+        <v>0.264</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.578</v>
+        <v>0.537</v>
       </c>
       <c r="AD15" t="n">
-        <v>11.7</v>
+        <v>0.576</v>
       </c>
       <c r="AE15" t="n">
-        <v>23.8</v>
+        <v>13.1</v>
       </c>
       <c r="AF15" t="n">
-        <v>80.09999999999999</v>
+        <v>25.7</v>
       </c>
       <c r="AG15" t="n">
-        <v>0.192</v>
+        <v>75.2</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>0.271</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>13</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>47</v>
       </c>
-      <c r="F16" t="n">
-        <v>97.5</v>
-      </c>
       <c r="G16" t="n">
-        <v>116.9</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="H16" t="n">
-        <v>113.8</v>
+        <v>113.4</v>
       </c>
       <c r="I16" t="n">
-        <v>0.574</v>
+        <v>111.3</v>
       </c>
       <c r="J16" t="n">
-        <v>10.7</v>
+        <v>0.577</v>
       </c>
       <c r="K16" t="n">
-        <v>0.826</v>
+        <v>13.3</v>
       </c>
       <c r="L16" t="n">
+        <v>0.759</v>
+      </c>
+      <c r="M16" t="n">
         <v>82</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>47</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>35</v>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>0.573</v>
       </c>
-      <c r="P16" t="n">
-        <v>3.05</v>
-      </c>
       <c r="Q16" t="n">
-        <v>-0.54</v>
+        <v>2.02</v>
       </c>
       <c r="R16" t="n">
-        <v>2.51</v>
+        <v>-0.55</v>
       </c>
       <c r="S16" t="n">
-        <v>97.5</v>
+        <v>1.48</v>
       </c>
       <c r="T16" t="n">
-        <v>116.9</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="U16" t="n">
-        <v>113.8</v>
+        <v>113.4</v>
       </c>
       <c r="V16" t="n">
-        <v>0.532</v>
+        <v>111.3</v>
       </c>
       <c r="W16" t="n">
-        <v>0.574</v>
+        <v>0.541</v>
       </c>
       <c r="X16" t="n">
-        <v>10.7</v>
+        <v>0.577</v>
       </c>
       <c r="Y16" t="n">
-        <v>24.8</v>
+        <v>13.3</v>
       </c>
       <c r="Z16" t="n">
-        <v>74.3</v>
+        <v>25.3</v>
       </c>
       <c r="AA16" t="n">
+        <v>78.09999999999999</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0.543</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.579</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>21.9</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="AH16" t="n">
         <v>0.264</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0.537</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0.576</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>13.1</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>25.7</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>75.2</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>0.271</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>14</v>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>ORL</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
         <v>47</v>
       </c>
-      <c r="F17" t="n">
-        <v>96.90000000000001</v>
-      </c>
       <c r="G17" t="n">
-        <v>113.4</v>
+        <v>101.7</v>
       </c>
       <c r="H17" t="n">
-        <v>111.3</v>
+        <v>121</v>
       </c>
       <c r="I17" t="n">
-        <v>0.577</v>
+        <v>118</v>
       </c>
       <c r="J17" t="n">
-        <v>13.3</v>
+        <v>0.606</v>
       </c>
       <c r="K17" t="n">
-        <v>0.759</v>
+        <v>11.3</v>
       </c>
       <c r="L17" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="M17" t="n">
         <v>82</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>47</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>35</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>0.573</v>
       </c>
-      <c r="P17" t="n">
-        <v>2.02</v>
-      </c>
       <c r="Q17" t="n">
-        <v>-0.55</v>
+        <v>3.05</v>
       </c>
       <c r="R17" t="n">
-        <v>1.48</v>
+        <v>-0.3</v>
       </c>
       <c r="S17" t="n">
-        <v>96.90000000000001</v>
+        <v>2.75</v>
       </c>
       <c r="T17" t="n">
-        <v>113.4</v>
+        <v>101.7</v>
       </c>
       <c r="U17" t="n">
-        <v>111.3</v>
+        <v>121</v>
       </c>
       <c r="V17" t="n">
-        <v>0.541</v>
+        <v>118</v>
       </c>
       <c r="W17" t="n">
-        <v>0.577</v>
+        <v>0.578</v>
       </c>
       <c r="X17" t="n">
-        <v>13.3</v>
+        <v>0.606</v>
       </c>
       <c r="Y17" t="n">
-        <v>25.3</v>
+        <v>11.3</v>
       </c>
       <c r="Z17" t="n">
-        <v>78.09999999999999</v>
+        <v>23.8</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.287</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.543</v>
+        <v>0.222</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.579</v>
+        <v>0.556</v>
       </c>
       <c r="AD17" t="n">
-        <v>13.8</v>
+        <v>0.594</v>
       </c>
       <c r="AE17" t="n">
-        <v>21.9</v>
+        <v>12.1</v>
       </c>
       <c r="AF17" t="n">
-        <v>74.7</v>
+        <v>25.9</v>
       </c>
       <c r="AG17" t="n">
-        <v>0.264</v>
+        <v>76.2</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>0.289</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>15</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>IND</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>47</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
       </c>
       <c r="F18" t="n">
-        <v>101.7</v>
+        <v>46</v>
       </c>
       <c r="G18" t="n">
-        <v>121</v>
+        <v>98.8</v>
       </c>
       <c r="H18" t="n">
-        <v>118</v>
+        <v>116.9</v>
       </c>
       <c r="I18" t="n">
-        <v>0.606</v>
+        <v>115.2</v>
       </c>
       <c r="J18" t="n">
-        <v>11.3</v>
+        <v>0.582</v>
       </c>
       <c r="K18" t="n">
-        <v>0.782</v>
+        <v>11.6</v>
       </c>
       <c r="L18" t="n">
+        <v>0.745</v>
+      </c>
+      <c r="M18" t="n">
         <v>82</v>
       </c>
-      <c r="M18" t="n">
-        <v>47</v>
-      </c>
       <c r="N18" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="O18" t="n">
-        <v>0.573</v>
+        <v>36</v>
       </c>
       <c r="P18" t="n">
-        <v>3.05</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.3</v>
+        <v>1.74</v>
       </c>
       <c r="R18" t="n">
-        <v>2.75</v>
+        <v>0.55</v>
       </c>
       <c r="S18" t="n">
-        <v>101.7</v>
+        <v>2.29</v>
       </c>
       <c r="T18" t="n">
-        <v>121</v>
+        <v>98.8</v>
       </c>
       <c r="U18" t="n">
-        <v>118</v>
+        <v>116.9</v>
       </c>
       <c r="V18" t="n">
-        <v>0.578</v>
+        <v>115.2</v>
       </c>
       <c r="W18" t="n">
-        <v>0.606</v>
+        <v>0.556</v>
       </c>
       <c r="X18" t="n">
-        <v>11.3</v>
+        <v>0.582</v>
       </c>
       <c r="Y18" t="n">
-        <v>23.8</v>
+        <v>11.6</v>
       </c>
       <c r="Z18" t="n">
-        <v>74.09999999999999</v>
+        <v>24.5</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.222</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.556</v>
+        <v>0.229</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.594</v>
+        <v>0.555</v>
       </c>
       <c r="AD18" t="n">
-        <v>12.1</v>
+        <v>0.592</v>
       </c>
       <c r="AE18" t="n">
-        <v>25.9</v>
+        <v>12.5</v>
       </c>
       <c r="AF18" t="n">
-        <v>76.2</v>
+        <v>21.6</v>
       </c>
       <c r="AG18" t="n">
-        <v>0.289</v>
+        <v>75.5</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>0.266</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>16</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>SAC</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
         <v>46</v>
       </c>
-      <c r="F19" t="n">
-        <v>98.8</v>
-      </c>
       <c r="G19" t="n">
-        <v>116.9</v>
+        <v>96.2</v>
       </c>
       <c r="H19" t="n">
-        <v>115.2</v>
+        <v>114</v>
       </c>
       <c r="I19" t="n">
-        <v>0.582</v>
+        <v>112.2</v>
       </c>
       <c r="J19" t="n">
-        <v>11.6</v>
+        <v>0.578</v>
       </c>
       <c r="K19" t="n">
-        <v>0.745</v>
+        <v>11.7</v>
       </c>
       <c r="L19" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+      <c r="M19" t="n">
         <v>82</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>46</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>36</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
         <v>0.5610000000000001</v>
       </c>
-      <c r="P19" t="n">
-        <v>1.74</v>
-      </c>
       <c r="Q19" t="n">
-        <v>0.55</v>
+        <v>1.76</v>
       </c>
       <c r="R19" t="n">
-        <v>2.29</v>
+        <v>-0.66</v>
       </c>
       <c r="S19" t="n">
-        <v>98.8</v>
+        <v>1.1</v>
       </c>
       <c r="T19" t="n">
-        <v>116.9</v>
+        <v>96.2</v>
       </c>
       <c r="U19" t="n">
-        <v>115.2</v>
+        <v>114</v>
       </c>
       <c r="V19" t="n">
-        <v>0.556</v>
+        <v>112.2</v>
       </c>
       <c r="W19" t="n">
-        <v>0.582</v>
+        <v>0.538</v>
       </c>
       <c r="X19" t="n">
-        <v>11.6</v>
+        <v>0.578</v>
       </c>
       <c r="Y19" t="n">
-        <v>24.5</v>
+        <v>11.7</v>
       </c>
       <c r="Z19" t="n">
-        <v>78.40000000000001</v>
+        <v>21.8</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.229</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.555</v>
+        <v>0.257</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.592</v>
+        <v>0.543</v>
       </c>
       <c r="AD19" t="n">
-        <v>12.5</v>
+        <v>0.573</v>
       </c>
       <c r="AE19" t="n">
-        <v>21.6</v>
+        <v>12.7</v>
       </c>
       <c r="AF19" t="n">
-        <v>75.5</v>
+        <v>21.9</v>
       </c>
       <c r="AG19" t="n">
-        <v>0.266</v>
+        <v>78.2</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.223</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>17</v>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>MIA</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>GSW</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
         <v>46</v>
       </c>
-      <c r="F20" t="n">
-        <v>96.2</v>
-      </c>
       <c r="G20" t="n">
-        <v>114</v>
+        <v>99.2</v>
       </c>
       <c r="H20" t="n">
-        <v>112.2</v>
+        <v>117.8</v>
       </c>
       <c r="I20" t="n">
-        <v>0.578</v>
+        <v>115.2</v>
       </c>
       <c r="J20" t="n">
-        <v>11.7</v>
+        <v>0.586</v>
       </c>
       <c r="K20" t="n">
-        <v>0.8179999999999999</v>
+        <v>12.5</v>
       </c>
       <c r="L20" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="M20" t="n">
         <v>82</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>46</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>36</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>0.5610000000000001</v>
       </c>
-      <c r="P20" t="n">
-        <v>1.76</v>
-      </c>
       <c r="Q20" t="n">
-        <v>-0.66</v>
+        <v>2.61</v>
       </c>
       <c r="R20" t="n">
-        <v>1.1</v>
+        <v>0.16</v>
       </c>
       <c r="S20" t="n">
-        <v>96.2</v>
+        <v>2.77</v>
       </c>
       <c r="T20" t="n">
-        <v>114</v>
+        <v>99.2</v>
       </c>
       <c r="U20" t="n">
-        <v>112.2</v>
+        <v>117.8</v>
       </c>
       <c r="V20" t="n">
-        <v>0.538</v>
+        <v>115.2</v>
       </c>
       <c r="W20" t="n">
-        <v>0.578</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="X20" t="n">
-        <v>11.7</v>
+        <v>0.586</v>
       </c>
       <c r="Y20" t="n">
-        <v>21.8</v>
+        <v>12.5</v>
       </c>
       <c r="Z20" t="n">
-        <v>78.09999999999999</v>
+        <v>27.5</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.257</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.543</v>
+        <v>0.219</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.573</v>
+        <v>0.539</v>
       </c>
       <c r="AD20" t="n">
-        <v>12.7</v>
+        <v>0.574</v>
       </c>
       <c r="AE20" t="n">
-        <v>21.9</v>
+        <v>11.5</v>
       </c>
       <c r="AF20" t="n">
-        <v>78.2</v>
+        <v>23.9</v>
       </c>
       <c r="AG20" t="n">
-        <v>0.223</v>
+        <v>72.5</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0.248</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>18</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>GSW</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>46</v>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
       </c>
       <c r="F21" t="n">
-        <v>99.2</v>
+        <v>41</v>
       </c>
       <c r="G21" t="n">
-        <v>117.8</v>
+        <v>99</v>
       </c>
       <c r="H21" t="n">
-        <v>115.2</v>
+        <v>114.5</v>
       </c>
       <c r="I21" t="n">
-        <v>0.586</v>
+        <v>113.4</v>
       </c>
       <c r="J21" t="n">
-        <v>12.5</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="K21" t="n">
-        <v>0.78</v>
+        <v>11.2</v>
       </c>
       <c r="L21" t="n">
+        <v>0.773</v>
+      </c>
+      <c r="M21" t="n">
         <v>82</v>
       </c>
-      <c r="M21" t="n">
-        <v>46</v>
-      </c>
       <c r="N21" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="O21" t="n">
-        <v>0.5610000000000001</v>
+        <v>41</v>
       </c>
       <c r="P21" t="n">
-        <v>2.61</v>
+        <v>0.5</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.16</v>
+        <v>1.12</v>
       </c>
       <c r="R21" t="n">
-        <v>2.77</v>
+        <v>0.12</v>
       </c>
       <c r="S21" t="n">
-        <v>99.2</v>
+        <v>1.24</v>
       </c>
       <c r="T21" t="n">
-        <v>117.8</v>
+        <v>99</v>
       </c>
       <c r="U21" t="n">
-        <v>115.2</v>
+        <v>114.5</v>
       </c>
       <c r="V21" t="n">
-        <v>0.5570000000000001</v>
+        <v>113.4</v>
       </c>
       <c r="W21" t="n">
-        <v>0.586</v>
+        <v>0.529</v>
       </c>
       <c r="X21" t="n">
-        <v>12.5</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="Y21" t="n">
-        <v>27.5</v>
+        <v>11.2</v>
       </c>
       <c r="Z21" t="n">
-        <v>76.09999999999999</v>
+        <v>25.1</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.219</v>
+        <v>76</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.539</v>
+        <v>0.257</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.574</v>
+        <v>0.533</v>
       </c>
       <c r="AD21" t="n">
-        <v>11.5</v>
+        <v>0.571</v>
       </c>
       <c r="AE21" t="n">
-        <v>23.9</v>
+        <v>12.2</v>
       </c>
       <c r="AF21" t="n">
-        <v>72.5</v>
+        <v>24</v>
       </c>
       <c r="AG21" t="n">
-        <v>0.248</v>
+        <v>74.90000000000001</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>0.286</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>19</v>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>HOU</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>41</v>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
       </c>
       <c r="F22" t="n">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="G22" t="n">
-        <v>114.5</v>
+        <v>96.3</v>
       </c>
       <c r="H22" t="n">
-        <v>113.4</v>
+        <v>114.9</v>
       </c>
       <c r="I22" t="n">
-        <v>0.5649999999999999</v>
+        <v>116.3</v>
       </c>
       <c r="J22" t="n">
-        <v>11.2</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="K22" t="n">
-        <v>0.773</v>
+        <v>11</v>
       </c>
       <c r="L22" t="n">
+        <v>0.791</v>
+      </c>
+      <c r="M22" t="n">
         <v>82</v>
       </c>
-      <c r="M22" t="n">
-        <v>41</v>
-      </c>
       <c r="N22" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O22" t="n">
-        <v>0.5</v>
+        <v>43</v>
       </c>
       <c r="P22" t="n">
-        <v>1.12</v>
+        <v>0.476</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.12</v>
+        <v>-1.44</v>
       </c>
       <c r="R22" t="n">
-        <v>1.24</v>
+        <v>-0.33</v>
       </c>
       <c r="S22" t="n">
-        <v>99</v>
+        <v>-1.77</v>
       </c>
       <c r="T22" t="n">
-        <v>114.5</v>
+        <v>96.3</v>
       </c>
       <c r="U22" t="n">
-        <v>113.4</v>
+        <v>114.9</v>
       </c>
       <c r="V22" t="n">
-        <v>0.529</v>
+        <v>116.3</v>
       </c>
       <c r="W22" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.534</v>
       </c>
       <c r="X22" t="n">
-        <v>11.2</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="Y22" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z22" t="n">
         <v>25.1</v>
       </c>
-      <c r="Z22" t="n">
-        <v>76</v>
-      </c>
       <c r="AA22" t="n">
-        <v>0.257</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.533</v>
+        <v>0.236</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.571</v>
+        <v>0.556</v>
       </c>
       <c r="AD22" t="n">
-        <v>12.2</v>
+        <v>0.589</v>
       </c>
       <c r="AE22" t="n">
-        <v>24</v>
+        <v>12.7</v>
       </c>
       <c r="AF22" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="AG22" t="n">
         <v>74.90000000000001</v>
       </c>
-      <c r="AG22" t="n">
-        <v>0.286</v>
+      <c r="AH22" t="n">
+        <v>0.251</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>20</v>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>CHI</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>39</v>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
       </c>
       <c r="F23" t="n">
-        <v>96.3</v>
+        <v>36</v>
       </c>
       <c r="G23" t="n">
-        <v>114.9</v>
+        <v>100.1</v>
       </c>
       <c r="H23" t="n">
-        <v>116.3</v>
+        <v>117.2</v>
       </c>
       <c r="I23" t="n">
-        <v>0.5679999999999999</v>
+        <v>119.4</v>
       </c>
       <c r="J23" t="n">
-        <v>11</v>
+        <v>0.576</v>
       </c>
       <c r="K23" t="n">
-        <v>0.791</v>
+        <v>11.6</v>
       </c>
       <c r="L23" t="n">
+        <v>0.797</v>
+      </c>
+      <c r="M23" t="n">
         <v>82</v>
       </c>
-      <c r="M23" t="n">
-        <v>39</v>
-      </c>
       <c r="N23" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="O23" t="n">
-        <v>0.476</v>
+        <v>46</v>
       </c>
       <c r="P23" t="n">
-        <v>-1.44</v>
+        <v>0.439</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.33</v>
+        <v>-2.18</v>
       </c>
       <c r="R23" t="n">
-        <v>-1.77</v>
+        <v>-0.19</v>
       </c>
       <c r="S23" t="n">
-        <v>96.3</v>
+        <v>-2.38</v>
       </c>
       <c r="T23" t="n">
-        <v>114.9</v>
+        <v>100.1</v>
       </c>
       <c r="U23" t="n">
-        <v>116.3</v>
+        <v>117.2</v>
       </c>
       <c r="V23" t="n">
-        <v>0.534</v>
+        <v>119.4</v>
       </c>
       <c r="W23" t="n">
-        <v>0.5679999999999999</v>
+        <v>0.539</v>
       </c>
       <c r="X23" t="n">
-        <v>11</v>
+        <v>0.576</v>
       </c>
       <c r="Y23" t="n">
-        <v>25.1</v>
+        <v>11.6</v>
       </c>
       <c r="Z23" t="n">
-        <v>76.40000000000001</v>
+        <v>27.1</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.236</v>
+        <v>75.2</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.556</v>
+        <v>0.251</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.589</v>
+        <v>0.572</v>
       </c>
       <c r="AD23" t="n">
-        <v>12.7</v>
+        <v>0.604</v>
       </c>
       <c r="AE23" t="n">
-        <v>23.6</v>
+        <v>12.4</v>
       </c>
       <c r="AF23" t="n">
-        <v>74.90000000000001</v>
+        <v>24.8</v>
       </c>
       <c r="AG23" t="n">
-        <v>0.251</v>
+        <v>72.90000000000001</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>0.242</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>21</v>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>ATL</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>36</v>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>BRK</t>
+        </is>
       </c>
       <c r="F24" t="n">
-        <v>100.1</v>
+        <v>32</v>
       </c>
       <c r="G24" t="n">
-        <v>117.2</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="H24" t="n">
-        <v>119.4</v>
+        <v>113.2</v>
       </c>
       <c r="I24" t="n">
-        <v>0.576</v>
+        <v>116.1</v>
       </c>
       <c r="J24" t="n">
-        <v>11.6</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="K24" t="n">
-        <v>0.797</v>
+        <v>11.8</v>
       </c>
       <c r="L24" t="n">
+        <v>0.756</v>
+      </c>
+      <c r="M24" t="n">
         <v>82</v>
       </c>
-      <c r="M24" t="n">
-        <v>36</v>
-      </c>
       <c r="N24" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O24" t="n">
-        <v>0.439</v>
+        <v>50</v>
       </c>
       <c r="P24" t="n">
-        <v>-2.18</v>
+        <v>0.39</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.19</v>
+        <v>-2.89</v>
       </c>
       <c r="R24" t="n">
-        <v>-2.38</v>
+        <v>-0.13</v>
       </c>
       <c r="S24" t="n">
-        <v>100.1</v>
+        <v>-3.02</v>
       </c>
       <c r="T24" t="n">
-        <v>117.2</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="U24" t="n">
-        <v>119.4</v>
+        <v>113.2</v>
       </c>
       <c r="V24" t="n">
-        <v>0.539</v>
+        <v>116.1</v>
       </c>
       <c r="W24" t="n">
-        <v>0.576</v>
+        <v>0.531</v>
       </c>
       <c r="X24" t="n">
-        <v>11.6</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="Y24" t="n">
-        <v>27.1</v>
+        <v>11.8</v>
       </c>
       <c r="Z24" t="n">
-        <v>75.2</v>
+        <v>25.2</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.251</v>
+        <v>76</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.572</v>
+        <v>0.234</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.604</v>
+        <v>0.543</v>
       </c>
       <c r="AD24" t="n">
-        <v>12.4</v>
+        <v>0.579</v>
       </c>
       <c r="AE24" t="n">
-        <v>24.8</v>
+        <v>11.4</v>
       </c>
       <c r="AF24" t="n">
-        <v>72.90000000000001</v>
+        <v>24</v>
       </c>
       <c r="AG24" t="n">
-        <v>0.242</v>
+        <v>74.8</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>0.239</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>22</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>BRK</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>32</v>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
       </c>
       <c r="F25" t="n">
-        <v>96.90000000000001</v>
+        <v>31</v>
       </c>
       <c r="G25" t="n">
-        <v>113.2</v>
+        <v>99.5</v>
       </c>
       <c r="H25" t="n">
-        <v>116.1</v>
+        <v>115.5</v>
       </c>
       <c r="I25" t="n">
-        <v>0.5610000000000001</v>
+        <v>120.4</v>
       </c>
       <c r="J25" t="n">
-        <v>11.8</v>
+        <v>0.579</v>
       </c>
       <c r="K25" t="n">
-        <v>0.756</v>
+        <v>13.6</v>
       </c>
       <c r="L25" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="M25" t="n">
         <v>82</v>
       </c>
-      <c r="M25" t="n">
-        <v>32</v>
-      </c>
       <c r="N25" t="n">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="O25" t="n">
-        <v>0.39</v>
+        <v>51</v>
       </c>
       <c r="P25" t="n">
-        <v>-2.89</v>
+        <v>0.378</v>
       </c>
       <c r="Q25" t="n">
-        <v>-0.13</v>
+        <v>-4.89</v>
       </c>
       <c r="R25" t="n">
-        <v>-3.02</v>
+        <v>0.68</v>
       </c>
       <c r="S25" t="n">
-        <v>96.90000000000001</v>
+        <v>-4.22</v>
       </c>
       <c r="T25" t="n">
-        <v>113.2</v>
+        <v>99.5</v>
       </c>
       <c r="U25" t="n">
-        <v>116.1</v>
+        <v>115.5</v>
       </c>
       <c r="V25" t="n">
-        <v>0.531</v>
+        <v>120.4</v>
       </c>
       <c r="W25" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.539</v>
       </c>
       <c r="X25" t="n">
-        <v>11.8</v>
+        <v>0.579</v>
       </c>
       <c r="Y25" t="n">
-        <v>25.2</v>
+        <v>13.6</v>
       </c>
       <c r="Z25" t="n">
-        <v>76</v>
+        <v>28.1</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.234</v>
+        <v>75.2</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.543</v>
+        <v>0.251</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.579</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="AD25" t="n">
-        <v>11.4</v>
+        <v>0.596</v>
       </c>
       <c r="AE25" t="n">
-        <v>24</v>
+        <v>10.9</v>
       </c>
       <c r="AF25" t="n">
-        <v>74.8</v>
+        <v>24.8</v>
       </c>
       <c r="AG25" t="n">
-        <v>0.239</v>
+        <v>71.90000000000001</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>0.235</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>23</v>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>UTA</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>31</v>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
       </c>
       <c r="F26" t="n">
-        <v>99.5</v>
+        <v>27</v>
       </c>
       <c r="G26" t="n">
-        <v>115.5</v>
+        <v>98.2</v>
       </c>
       <c r="H26" t="n">
-        <v>120.4</v>
+        <v>107.2</v>
       </c>
       <c r="I26" t="n">
-        <v>0.579</v>
+        <v>114.3</v>
       </c>
       <c r="J26" t="n">
-        <v>13.6</v>
+        <v>0.543</v>
       </c>
       <c r="K26" t="n">
-        <v>0.83</v>
+        <v>13.4</v>
       </c>
       <c r="L26" t="n">
+        <v>0.764</v>
+      </c>
+      <c r="M26" t="n">
         <v>82</v>
       </c>
-      <c r="M26" t="n">
-        <v>31</v>
-      </c>
       <c r="N26" t="n">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="O26" t="n">
-        <v>0.378</v>
+        <v>55</v>
       </c>
       <c r="P26" t="n">
-        <v>-4.89</v>
+        <v>0.329</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.68</v>
+        <v>-7</v>
       </c>
       <c r="R26" t="n">
-        <v>-4.22</v>
+        <v>0.43</v>
       </c>
       <c r="S26" t="n">
-        <v>99.5</v>
+        <v>-6.57</v>
       </c>
       <c r="T26" t="n">
-        <v>115.5</v>
+        <v>98.2</v>
       </c>
       <c r="U26" t="n">
-        <v>120.4</v>
+        <v>107.2</v>
       </c>
       <c r="V26" t="n">
-        <v>0.539</v>
+        <v>114.3</v>
       </c>
       <c r="W26" t="n">
-        <v>0.579</v>
+        <v>0.509</v>
       </c>
       <c r="X26" t="n">
-        <v>13.6</v>
+        <v>0.543</v>
       </c>
       <c r="Y26" t="n">
-        <v>28.1</v>
+        <v>13.4</v>
       </c>
       <c r="Z26" t="n">
-        <v>75.2</v>
+        <v>23.8</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.251</v>
+        <v>74.8</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.238</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.596</v>
+        <v>0.551</v>
       </c>
       <c r="AD26" t="n">
-        <v>10.9</v>
+        <v>0.585</v>
       </c>
       <c r="AE26" t="n">
-        <v>24.8</v>
+        <v>13.5</v>
       </c>
       <c r="AF26" t="n">
-        <v>71.90000000000001</v>
+        <v>25.2</v>
       </c>
       <c r="AG26" t="n">
-        <v>0.235</v>
+        <v>76.2</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>24</v>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>MEM</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>27</v>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
       </c>
       <c r="F27" t="n">
-        <v>98.2</v>
+        <v>25</v>
       </c>
       <c r="G27" t="n">
-        <v>107.2</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="H27" t="n">
-        <v>114.3</v>
+        <v>112.3</v>
       </c>
       <c r="I27" t="n">
-        <v>0.543</v>
+        <v>118.8</v>
       </c>
       <c r="J27" t="n">
-        <v>13.4</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="K27" t="n">
-        <v>0.764</v>
+        <v>12.4</v>
       </c>
       <c r="L27" t="n">
+        <v>0.756</v>
+      </c>
+      <c r="M27" t="n">
         <v>82</v>
       </c>
-      <c r="M27" t="n">
-        <v>27</v>
-      </c>
       <c r="N27" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="O27" t="n">
-        <v>0.329</v>
+        <v>57</v>
       </c>
       <c r="P27" t="n">
-        <v>-7</v>
+        <v>0.305</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.43</v>
+        <v>-6.44</v>
       </c>
       <c r="R27" t="n">
-        <v>-6.57</v>
+        <v>-0.01</v>
       </c>
       <c r="S27" t="n">
-        <v>98.2</v>
+        <v>-6.45</v>
       </c>
       <c r="T27" t="n">
-        <v>107.2</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="U27" t="n">
-        <v>114.3</v>
+        <v>112.3</v>
       </c>
       <c r="V27" t="n">
-        <v>0.509</v>
+        <v>118.8</v>
       </c>
       <c r="W27" t="n">
-        <v>0.543</v>
+        <v>0.535</v>
       </c>
       <c r="X27" t="n">
-        <v>13.4</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="Y27" t="n">
-        <v>23.8</v>
+        <v>12.4</v>
       </c>
       <c r="Z27" t="n">
-        <v>74.8</v>
+        <v>24.2</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.238</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.551</v>
+        <v>0.241</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.585</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="AD27" t="n">
-        <v>13.5</v>
+        <v>0.595</v>
       </c>
       <c r="AE27" t="n">
-        <v>25.2</v>
+        <v>12.2</v>
       </c>
       <c r="AF27" t="n">
-        <v>76.2</v>
+        <v>26.1</v>
       </c>
       <c r="AG27" t="n">
-        <v>0.25</v>
+        <v>75.8</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0.218</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>25</v>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>TOR</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>25</v>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
       </c>
       <c r="F28" t="n">
-        <v>99.40000000000001</v>
+        <v>22</v>
       </c>
       <c r="G28" t="n">
-        <v>112.3</v>
+        <v>101.1</v>
       </c>
       <c r="H28" t="n">
-        <v>118.8</v>
+        <v>110</v>
       </c>
       <c r="I28" t="n">
-        <v>0.5659999999999999</v>
+        <v>116.4</v>
       </c>
       <c r="J28" t="n">
-        <v>12.4</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="K28" t="n">
-        <v>0.756</v>
+        <v>13.2</v>
       </c>
       <c r="L28" t="n">
+        <v>0.782</v>
+      </c>
+      <c r="M28" t="n">
         <v>82</v>
       </c>
-      <c r="M28" t="n">
-        <v>25</v>
-      </c>
       <c r="N28" t="n">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="O28" t="n">
-        <v>0.305</v>
+        <v>60</v>
       </c>
       <c r="P28" t="n">
-        <v>-6.44</v>
+        <v>0.268</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.01</v>
+        <v>-6.49</v>
       </c>
       <c r="R28" t="n">
-        <v>-6.45</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="S28" t="n">
-        <v>99.40000000000001</v>
+        <v>-5.8</v>
       </c>
       <c r="T28" t="n">
-        <v>112.3</v>
+        <v>101.1</v>
       </c>
       <c r="U28" t="n">
-        <v>118.8</v>
+        <v>110</v>
       </c>
       <c r="V28" t="n">
-        <v>0.535</v>
+        <v>116.4</v>
       </c>
       <c r="W28" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.532</v>
       </c>
       <c r="X28" t="n">
-        <v>12.4</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="Y28" t="n">
-        <v>24.2</v>
+        <v>13.2</v>
       </c>
       <c r="Z28" t="n">
-        <v>73.90000000000001</v>
+        <v>22.9</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.241</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.22</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.595</v>
+        <v>0.555</v>
       </c>
       <c r="AD28" t="n">
-        <v>12.2</v>
+        <v>0.585</v>
       </c>
       <c r="AE28" t="n">
-        <v>26.1</v>
+        <v>11.7</v>
       </c>
       <c r="AF28" t="n">
-        <v>75.8</v>
+        <v>23.6</v>
       </c>
       <c r="AG28" t="n">
-        <v>0.218</v>
+        <v>77.09999999999999</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>0.222</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>26</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>22</v>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>CHO</t>
+        </is>
       </c>
       <c r="F29" t="n">
-        <v>101.1</v>
+        <v>21</v>
       </c>
       <c r="G29" t="n">
-        <v>110</v>
+        <v>97.3</v>
       </c>
       <c r="H29" t="n">
-        <v>116.4</v>
+        <v>109.3</v>
       </c>
       <c r="I29" t="n">
-        <v>0.5629999999999999</v>
+        <v>119.8</v>
       </c>
       <c r="J29" t="n">
-        <v>13.2</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="K29" t="n">
-        <v>0.782</v>
+        <v>12.6</v>
       </c>
       <c r="L29" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="M29" t="n">
         <v>82</v>
       </c>
-      <c r="M29" t="n">
-        <v>22</v>
-      </c>
       <c r="N29" t="n">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="O29" t="n">
-        <v>0.268</v>
+        <v>61</v>
       </c>
       <c r="P29" t="n">
-        <v>-6.49</v>
+        <v>0.256</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.6899999999999999</v>
+        <v>-10.24</v>
       </c>
       <c r="R29" t="n">
-        <v>-5.8</v>
+        <v>0.13</v>
       </c>
       <c r="S29" t="n">
-        <v>101.1</v>
+        <v>-10.12</v>
       </c>
       <c r="T29" t="n">
-        <v>110</v>
+        <v>97.3</v>
       </c>
       <c r="U29" t="n">
-        <v>116.4</v>
+        <v>109.3</v>
       </c>
       <c r="V29" t="n">
-        <v>0.532</v>
+        <v>119.8</v>
       </c>
       <c r="W29" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.529</v>
       </c>
       <c r="X29" t="n">
-        <v>13.2</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="Y29" t="n">
-        <v>22.9</v>
+        <v>12.6</v>
       </c>
       <c r="Z29" t="n">
-        <v>76.40000000000001</v>
+        <v>21.1</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.22</v>
+        <v>74.5</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.555</v>
+        <v>0.212</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.585</v>
+        <v>0.572</v>
       </c>
       <c r="AD29" t="n">
-        <v>11.7</v>
+        <v>0.603</v>
       </c>
       <c r="AE29" t="n">
-        <v>23.6</v>
+        <v>12.3</v>
       </c>
       <c r="AF29" t="n">
-        <v>77.09999999999999</v>
+        <v>25.5</v>
       </c>
       <c r="AG29" t="n">
-        <v>0.222</v>
+        <v>78.90000000000001</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>0.236</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>27</v>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>CHO</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
         <v>21</v>
       </c>
-      <c r="F30" t="n">
-        <v>97.3</v>
-      </c>
       <c r="G30" t="n">
-        <v>109.3</v>
+        <v>97.2</v>
       </c>
       <c r="H30" t="n">
-        <v>119.8</v>
+        <v>108.3</v>
       </c>
       <c r="I30" t="n">
-        <v>0.5600000000000001</v>
+        <v>117.5</v>
       </c>
       <c r="J30" t="n">
-        <v>12.6</v>
+        <v>0.539</v>
       </c>
       <c r="K30" t="n">
-        <v>0.786</v>
+        <v>13.4</v>
       </c>
       <c r="L30" t="n">
+        <v>0.791</v>
+      </c>
+      <c r="M30" t="n">
         <v>82</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>21</v>
       </c>
-      <c r="N30" t="n">
+      <c r="O30" t="n">
         <v>61</v>
       </c>
-      <c r="O30" t="n">
+      <c r="P30" t="n">
         <v>0.256</v>
       </c>
-      <c r="P30" t="n">
-        <v>-10.24</v>
-      </c>
       <c r="Q30" t="n">
-        <v>0.13</v>
+        <v>-9.02</v>
       </c>
       <c r="R30" t="n">
-        <v>-10.12</v>
+        <v>0.74</v>
       </c>
       <c r="S30" t="n">
-        <v>97.3</v>
+        <v>-8.289999999999999</v>
       </c>
       <c r="T30" t="n">
-        <v>109.3</v>
+        <v>97.2</v>
       </c>
       <c r="U30" t="n">
-        <v>119.8</v>
+        <v>108.3</v>
       </c>
       <c r="V30" t="n">
-        <v>0.529</v>
+        <v>117.5</v>
       </c>
       <c r="W30" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.503</v>
       </c>
       <c r="X30" t="n">
-        <v>12.6</v>
+        <v>0.539</v>
       </c>
       <c r="Y30" t="n">
-        <v>21.1</v>
+        <v>13.4</v>
       </c>
       <c r="Z30" t="n">
-        <v>74.5</v>
+        <v>27.5</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.212</v>
+        <v>74</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.572</v>
+        <v>0.228</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.603</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="AD30" t="n">
-        <v>12.3</v>
+        <v>0.595</v>
       </c>
       <c r="AE30" t="n">
-        <v>25.5</v>
+        <v>12.8</v>
       </c>
       <c r="AF30" t="n">
-        <v>78.90000000000001</v>
+        <v>26</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.236</v>
+        <v>72.5</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>0.273</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>28</v>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>POR</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>21</v>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
       </c>
       <c r="F31" t="n">
-        <v>97.2</v>
+        <v>15</v>
       </c>
       <c r="G31" t="n">
-        <v>108.3</v>
+        <v>102.7</v>
       </c>
       <c r="H31" t="n">
-        <v>117.5</v>
+        <v>110.5</v>
       </c>
       <c r="I31" t="n">
-        <v>0.539</v>
+        <v>119.6</v>
       </c>
       <c r="J31" t="n">
-        <v>13.4</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="K31" t="n">
-        <v>0.791</v>
+        <v>12.2</v>
       </c>
       <c r="L31" t="n">
+        <v>0.764</v>
+      </c>
+      <c r="M31" t="n">
         <v>82</v>
       </c>
-      <c r="M31" t="n">
-        <v>21</v>
-      </c>
       <c r="N31" t="n">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="O31" t="n">
-        <v>0.256</v>
+        <v>67</v>
       </c>
       <c r="P31" t="n">
-        <v>-9.02</v>
+        <v>0.183</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.74</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="R31" t="n">
-        <v>-8.289999999999999</v>
+        <v>0</v>
       </c>
       <c r="S31" t="n">
-        <v>97.2</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="T31" t="n">
-        <v>108.3</v>
+        <v>102.7</v>
       </c>
       <c r="U31" t="n">
-        <v>117.5</v>
+        <v>110.5</v>
       </c>
       <c r="V31" t="n">
-        <v>0.503</v>
+        <v>119.6</v>
       </c>
       <c r="W31" t="n">
-        <v>0.539</v>
+        <v>0.538</v>
       </c>
       <c r="X31" t="n">
-        <v>13.4</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="Y31" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>72.5</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.221</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>12</v>
+      </c>
+      <c r="AF31" t="n">
         <v>27.5</v>
       </c>
-      <c r="Z31" t="n">
-        <v>74</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>0.228</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>0.5580000000000001</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>0.595</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="AE31" t="n">
-        <v>26</v>
-      </c>
-      <c r="AF31" t="n">
-        <v>72.5</v>
-      </c>
       <c r="AG31" t="n">
-        <v>0.273</v>
+        <v>80</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0.258</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>29</v>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>2023-24</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>15</v>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
       </c>
       <c r="F32" t="n">
-        <v>102.7</v>
+        <v>14</v>
       </c>
       <c r="G32" t="n">
-        <v>110.5</v>
+        <v>99.8</v>
       </c>
       <c r="H32" t="n">
-        <v>119.6</v>
+        <v>109.7</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5669999999999999</v>
+        <v>118.8</v>
       </c>
       <c r="J32" t="n">
-        <v>12.2</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="K32" t="n">
-        <v>0.764</v>
+        <v>13.5</v>
       </c>
       <c r="L32" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="M32" t="n">
         <v>82</v>
       </c>
-      <c r="M32" t="n">
-        <v>15</v>
-      </c>
       <c r="N32" t="n">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="O32" t="n">
-        <v>0.183</v>
+        <v>68</v>
       </c>
       <c r="P32" t="n">
-        <v>-9.289999999999999</v>
+        <v>0.171</v>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>-9.109999999999999</v>
       </c>
       <c r="R32" t="n">
-        <v>-9.289999999999999</v>
+        <v>0.05</v>
       </c>
       <c r="S32" t="n">
-        <v>102.7</v>
+        <v>-9.06</v>
       </c>
       <c r="T32" t="n">
-        <v>110.5</v>
+        <v>99.8</v>
       </c>
       <c r="U32" t="n">
-        <v>119.6</v>
+        <v>109.7</v>
       </c>
       <c r="V32" t="n">
-        <v>0.538</v>
+        <v>118.8</v>
       </c>
       <c r="W32" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.526</v>
       </c>
       <c r="X32" t="n">
-        <v>12.2</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="Y32" t="n">
-        <v>20</v>
+        <v>13.5</v>
       </c>
       <c r="Z32" t="n">
-        <v>72.5</v>
+        <v>23.9</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.221</v>
+        <v>77.3</v>
       </c>
       <c r="AB32" t="n">
-        <v>0.5620000000000001</v>
+        <v>0.246</v>
       </c>
       <c r="AC32" t="n">
-        <v>0.595</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="AD32" t="n">
-        <v>12</v>
+        <v>0.596</v>
       </c>
       <c r="AE32" t="n">
-        <v>27.5</v>
+        <v>11.1</v>
       </c>
       <c r="AF32" t="n">
-        <v>80</v>
+        <v>22.7</v>
       </c>
       <c r="AG32" t="n">
-        <v>0.258</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B33" t="n">
-        <v>30</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>2023-24</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>DET</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>14</v>
-      </c>
-      <c r="F33" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="G33" t="n">
-        <v>109.7</v>
-      </c>
-      <c r="H33" t="n">
-        <v>118.8</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="J33" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="L33" t="n">
-        <v>82</v>
-      </c>
-      <c r="M33" t="n">
-        <v>14</v>
-      </c>
-      <c r="N33" t="n">
-        <v>68</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0.171</v>
-      </c>
-      <c r="P33" t="n">
-        <v>-9.109999999999999</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="R33" t="n">
-        <v>-9.06</v>
-      </c>
-      <c r="S33" t="n">
-        <v>99.8</v>
-      </c>
-      <c r="T33" t="n">
-        <v>109.7</v>
-      </c>
-      <c r="U33" t="n">
-        <v>118.8</v>
-      </c>
-      <c r="V33" t="n">
-        <v>0.526</v>
-      </c>
-      <c r="W33" t="n">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="X33" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>23.9</v>
-      </c>
-      <c r="Z33" t="n">
-        <v>77.3</v>
-      </c>
-      <c r="AA33" t="n">
-        <v>0.246</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>0.5580000000000001</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>0.596</v>
-      </c>
-      <c r="AD33" t="n">
-        <v>11.1</v>
-      </c>
-      <c r="AE33" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="AF33" t="n">
         <v>76.09999999999999</v>
       </c>
-      <c r="AG33" t="n">
+      <c r="AH32" t="n">
         <v>0.276</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="AD1:AG1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>